<commit_message>
executed the complete flow once to test everything is working proper or not
</commit_message>
<xml_diff>
--- a/Essen/src/test/java/com/essen/testData/LoginData.xlsx
+++ b/Essen/src/test/java/com/essen/testData/LoginData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369A525F-AB5A-4AE9-943D-B206241F33BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B7D128-30DE-480F-8BE8-953F3A7D14AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="0" windowWidth="16332" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <t>anadkarni@essenmed.com</t>
   </si>
   <si>
-    <t>Bronx@1990</t>
+    <t>Bronx@1995</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
New changes added as timestamp
</commit_message>
<xml_diff>
--- a/Essen/src/test/java/com/essen/testData/LoginData.xlsx
+++ b/Essen/src/test/java/com/essen/testData/LoginData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA58EB5-F3F5-4E13-BFA0-92B1A438652F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD939B9-68BC-40B7-8B70-9E07251EF520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -37,10 +37,13 @@
     <t>Pass$123</t>
   </si>
   <si>
-    <t>aditya2</t>
-  </si>
-  <si>
     <t>aditya905</t>
+  </si>
+  <si>
+    <t>adityatest3</t>
+  </si>
+  <si>
+    <t>adityatest1</t>
   </si>
 </sst>
 </file>
@@ -439,7 +442,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,7 +461,7 @@
     </row>
     <row r="2" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -474,7 +477,7 @@
     </row>
     <row r="4" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -482,7 +485,7 @@
     </row>
     <row r="5" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>

</xml_diff>